<commit_message>
Exp module for input & test-1
</commit_message>
<xml_diff>
--- a/migforecasting/less100/inputcheck.xlsx
+++ b/migforecasting/less100/inputcheck.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="ThisYear" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +973,7 @@
       <c r="Q9" s="2">
         <v>1051.3399999999999</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="5">
         <f t="shared" si="0"/>
         <v>839.33999999999992</v>
       </c>

</xml_diff>